<commit_message>
added weight column for more simple usage
</commit_message>
<xml_diff>
--- a/account_info.xlsx
+++ b/account_info.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2BA132-12CA-471F-88C3-FD87DB957811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC8A72D-6AB2-4504-9B93-657CDE5C0D87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="38">
   <si>
     <t>T</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>roth</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13:C30"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +485,7 @@
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -498,8 +501,11 @@
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -515,8 +521,11 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -532,8 +541,11 @@
       <c r="E3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -549,8 +561,11 @@
       <c r="E4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -566,8 +581,11 @@
       <c r="E5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -583,8 +601,11 @@
       <c r="E6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -600,8 +621,11 @@
       <c r="E7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -617,8 +641,11 @@
       <c r="E8">
         <v>200</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -634,8 +661,11 @@
       <c r="E9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -651,8 +681,11 @@
       <c r="E10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -668,8 +701,11 @@
       <c r="E11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -685,8 +721,11 @@
       <c r="E12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -702,8 +741,11 @@
       <c r="E13">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -719,8 +761,11 @@
       <c r="E14">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -736,8 +781,11 @@
       <c r="E15">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -752,6 +800,9 @@
       </c>
       <c r="E16">
         <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -770,6 +821,9 @@
       <c r="E17">
         <v>130</v>
       </c>
+      <c r="F17">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -787,6 +841,9 @@
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -804,6 +861,9 @@
       <c r="E19">
         <v>1500</v>
       </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -821,6 +881,9 @@
       <c r="E20">
         <v>140</v>
       </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -838,6 +901,9 @@
       <c r="E21">
         <v>3600</v>
       </c>
+      <c r="F21">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -855,6 +921,9 @@
       <c r="E22">
         <v>100</v>
       </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -872,6 +941,10 @@
       <c r="E23">
         <v>500</v>
       </c>
+      <c r="F23">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -889,6 +962,10 @@
       <c r="E24">
         <v>90</v>
       </c>
+      <c r="F24">
+        <f t="shared" ref="F24:F30" si="0">1/8</f>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -906,6 +983,10 @@
       <c r="E25">
         <v>90</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -923,6 +1004,10 @@
       <c r="E26">
         <v>900</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -940,6 +1025,10 @@
       <c r="E27">
         <v>6</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -957,6 +1046,10 @@
       <c r="E28">
         <v>900</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -974,6 +1067,10 @@
       <c r="E29">
         <v>150</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -990,6 +1087,10 @@
       </c>
       <c r="E30">
         <v>20</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>